<commit_message>
Added environmental KPIs for oil refinery UCs
</commit_message>
<xml_diff>
--- a/models_inputs/models_input_parameters/parameters_guide.xlsx
+++ b/models_inputs/models_input_parameters/parameters_guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epuntuagr-my.sharepoint.com/personal/hkoutalidis_epu_ntua_gr/Documents/Enershare/Paper 2 H2 scenaros paper/Dummy_environment_dir/models_inputs/models_input_parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epuntuagr-my.sharepoint.com/personal/hkoutalidis_epu_ntua_gr/Documents/Enershare/Paper 2 H2 scenaros paper/P2G_Hydrogen_Repository_remote/models_inputs/models_input_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F636F3EF-83C6-4876-93AD-9A1831E0898D}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80053391-DBC9-48A0-9C2B-EAAFF791116B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulations S2.1 (own RES inve)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Main (2024)</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Var Opex (EUR/MWh)</t>
+  </si>
+  <si>
+    <t>Max injection ratio (Natural gas grid exit point UC)</t>
   </si>
 </sst>
 </file>
@@ -273,10 +276,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +918,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B32" s="8">
         <v>0.1</v>
@@ -956,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26B971-9089-40B6-B7D9-B4FE2F3EF079}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added LCOH computation, printing and exporting
</commit_message>
<xml_diff>
--- a/models_inputs/models_input_parameters/parameters_guide.xlsx
+++ b/models_inputs/models_input_parameters/parameters_guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epuntuagr-my.sharepoint.com/personal/hkoutalidis_epu_ntua_gr/Documents/Enershare/Paper 2 H2 scenarios paper/P2G_Hydrogen_Repository_remote/models_inputs/models_input_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88010F9D-B8C8-4091-84EE-1DF4352180B3}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34F6ABD6-5F7B-4A1D-AAF8-91FF6A6559DC}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="12825" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulations S2.1 (own RES inve)" sheetId="1" r:id="rId1"/>
@@ -553,418 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>409000</v>
-      </c>
-      <c r="C3">
-        <f>B3*0.95</f>
-        <v>388550</v>
-      </c>
-      <c r="D3">
-        <f>B3*0.9</f>
-        <v>368100</v>
-      </c>
-      <c r="E3">
-        <f>B3*0.8</f>
-        <v>327200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C9" si="0">B4*0.95</f>
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D9" si="1">B4*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E9" si="2">B4*0.8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>27400</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>26030</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>24660</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>21920</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>272000</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>258400</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>244800</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>217600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>15250</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>14487.5</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>13725</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>12200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>550000</v>
-      </c>
-      <c r="C13">
-        <f>B13*0.95</f>
-        <v>522500</v>
-      </c>
-      <c r="D13">
-        <f>B13*0.9</f>
-        <v>495000</v>
-      </c>
-      <c r="E13">
-        <f>D13*0.8</f>
-        <v>396000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>13750</v>
-      </c>
-      <c r="C14">
-        <f>B14*0.95</f>
-        <v>13062.5</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14" si="3">B14*0.9</f>
-        <v>12375</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ref="E14" si="4">D14*0.8</f>
-        <v>9900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15">
-        <v>1.33</v>
-      </c>
-      <c r="C15">
-        <f>$B$15</f>
-        <v>1.33</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ref="D15" si="5">$B$15</f>
-        <v>1.33</v>
-      </c>
-      <c r="E15">
-        <f>$B$15</f>
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="C16">
-        <v>0.79</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0.82</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>7250</v>
-      </c>
-      <c r="C20">
-        <f>B20*0.95</f>
-        <v>6887.5</v>
-      </c>
-      <c r="D20">
-        <f>B20*0.9</f>
-        <v>6525</v>
-      </c>
-      <c r="E20">
-        <f>B20*0.8</f>
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>145</v>
-      </c>
-      <c r="C21">
-        <f>B21*0.95</f>
-        <v>137.75</v>
-      </c>
-      <c r="D21">
-        <f>B21*0.9</f>
-        <v>130.5</v>
-      </c>
-      <c r="E21">
-        <f>B21*0.8</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23">
-        <v>0.99</v>
-      </c>
-      <c r="C23">
-        <v>0.99</v>
-      </c>
-      <c r="D23">
-        <v>0.99</v>
-      </c>
-      <c r="E23">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>0.99</v>
-      </c>
-      <c r="C24">
-        <v>0.99</v>
-      </c>
-      <c r="D24">
-        <v>0.99</v>
-      </c>
-      <c r="E24">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="C32" s="8">
-        <v>0.12</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E32" s="10">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26B971-9089-40B6-B7D9-B4FE2F3EF079}">
-  <dimension ref="A1:E31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -997,6 +586,417 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>409000</v>
+      </c>
+      <c r="C3">
+        <f>B3*0.95</f>
+        <v>388550</v>
+      </c>
+      <c r="D3">
+        <f>B3*0.9</f>
+        <v>368100</v>
+      </c>
+      <c r="E3">
+        <f>B3*0.8</f>
+        <v>327200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C9" si="0">B4*0.95</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D9" si="1">B4*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E9" si="2">B4*0.8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>27400</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>26030</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>24660</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>21920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>272000</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>258400</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>244800</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>217600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>15250</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>14487.5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>13725</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>12200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>550000</v>
+      </c>
+      <c r="C13">
+        <f>B13*0.95</f>
+        <v>522500</v>
+      </c>
+      <c r="D13">
+        <f>B13*0.9</f>
+        <v>495000</v>
+      </c>
+      <c r="E13">
+        <f>D13*0.8</f>
+        <v>396000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13750</v>
+      </c>
+      <c r="C14">
+        <f>B14*0.95</f>
+        <v>13062.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="3">B14*0.9</f>
+        <v>12375</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="4">D14*0.8</f>
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>1.33</v>
+      </c>
+      <c r="C15">
+        <f>$B$15</f>
+        <v>1.33</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15" si="5">$B$15</f>
+        <v>1.33</v>
+      </c>
+      <c r="E15">
+        <f>$B$15</f>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.79</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>7250</v>
+      </c>
+      <c r="C20">
+        <f>B20*0.95</f>
+        <v>6887.5</v>
+      </c>
+      <c r="D20">
+        <f>B20*0.9</f>
+        <v>6525</v>
+      </c>
+      <c r="E20">
+        <f>B20*0.8</f>
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>145</v>
+      </c>
+      <c r="C21">
+        <f>B21*0.95</f>
+        <v>137.75</v>
+      </c>
+      <c r="D21">
+        <f>B21*0.9</f>
+        <v>130.5</v>
+      </c>
+      <c r="E21">
+        <f>B21*0.8</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>0.99</v>
+      </c>
+      <c r="C23">
+        <v>0.99</v>
+      </c>
+      <c r="D23">
+        <v>0.99</v>
+      </c>
+      <c r="E23">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>0.99</v>
+      </c>
+      <c r="C24">
+        <v>0.99</v>
+      </c>
+      <c r="D24">
+        <v>0.99</v>
+      </c>
+      <c r="E24">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26B971-9089-40B6-B7D9-B4FE2F3EF079}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -1180,13 +1180,13 @@
         <v>0.75600000000000001</v>
       </c>
       <c r="C16">
-        <v>0.79400000000000004</v>
+        <v>0.79</v>
       </c>
       <c r="D16" s="6">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="E16" s="6">
-        <v>0.81</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,19 +1199,19 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>11300</v>
+        <v>7250</v>
       </c>
       <c r="C19">
         <f>B19*0.95</f>
-        <v>10735</v>
+        <v>6887.5</v>
       </c>
       <c r="D19">
         <f>B19*0.9</f>
-        <v>10170</v>
+        <v>6525</v>
       </c>
       <c r="E19">
         <f>B19*0.8</f>
-        <v>9040</v>
+        <v>5800</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1219,19 +1219,19 @@
         <v>29</v>
       </c>
       <c r="B20">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="C20">
         <f>B20*0.95</f>
-        <v>213.75</v>
+        <v>137.75</v>
       </c>
       <c r="D20">
         <f>B20*0.9</f>
-        <v>202.5</v>
+        <v>130.5</v>
       </c>
       <c r="E20">
         <f>B20*0.8</f>
-        <v>180</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>